<commit_message>
Enhance cross plot functionality and update database queries
- Modify SQL query to order results by target_name for simulated well selection
- Adjust y-axis and x-axis tick intervals in cross plot for better visualization
- Update axis labels to reflect new units and improve clarity
- Add reference numbers to wells in the cross plot and Excel output
- Revise release notes in the HTML template to include recent changes
</commit_message>
<xml_diff>
--- a/app/database/stratigraphic.xlsx
+++ b/app/database/stratigraphic.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\steve\projects\offset-well-identification\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\steve\projects\afe\app\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544E226B-187D-4EE4-9F67-115BE3849CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1654A840-56D4-4131-B22D-92B5DB4AC1D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{5A26212E-1421-4DA3-B8E9-B09BBE008E54}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="90">
   <si>
     <t>Permian</t>
   </si>
@@ -257,9 +257,6 @@
     <t>#1f220a</t>
   </si>
   <si>
-    <t>#26a4b7</t>
-  </si>
-  <si>
     <t>#964401</t>
   </si>
   <si>
@@ -284,25 +281,31 @@
     <t>#03c893</t>
   </si>
   <si>
-    <t>#4c7832</t>
-  </si>
-  <si>
-    <t>#b15b27</t>
-  </si>
-  <si>
-    <t>#e37255</t>
-  </si>
-  <si>
-    <t>#98252a</t>
-  </si>
-  <si>
-    <t>#ef8877</t>
-  </si>
-  <si>
     <t>#1d5da6</t>
   </si>
   <si>
     <t>#2fb3e6</t>
+  </si>
+  <si>
+    <t>#CC0000</t>
+  </si>
+  <si>
+    <t>#B20000</t>
+  </si>
+  <si>
+    <t>#990000</t>
+  </si>
+  <si>
+    <t>#800000</t>
+  </si>
+  <si>
+    <t>#660000</t>
+  </si>
+  <si>
+    <t>#4D0000</t>
+  </si>
+  <si>
+    <t>#330000</t>
   </si>
 </sst>
 </file>
@@ -683,7 +686,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -783,7 +786,7 @@
         <v>3</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -809,7 +812,7 @@
         <v>4</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -835,7 +838,7 @@
         <v>5</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -861,7 +864,7 @@
         <v>6</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -887,7 +890,7 @@
         <v>7</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -913,7 +916,7 @@
         <v>8</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -939,7 +942,7 @@
         <v>9</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -965,7 +968,7 @@
         <v>10</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -988,7 +991,7 @@
         <v>11</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -1014,7 +1017,7 @@
         <v>12</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -1040,7 +1043,7 @@
         <v>13</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -1066,7 +1069,7 @@
         <v>14</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -1092,7 +1095,7 @@
         <v>15</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -1118,7 +1121,7 @@
         <v>16</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -1144,7 +1147,7 @@
         <v>17</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1170,7 +1173,7 @@
         <v>18</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -1196,7 +1199,7 @@
         <v>19</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update landing zone colors
</commit_message>
<xml_diff>
--- a/app/database/stratigraphic.xlsx
+++ b/app/database/stratigraphic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\steve\projects\afe\app\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1654A840-56D4-4131-B22D-92B5DB4AC1D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA97429-190B-4176-B60A-1CDB5FDE681B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{5A26212E-1421-4DA3-B8E9-B09BBE008E54}"/>
   </bookViews>
@@ -287,25 +287,25 @@
     <t>#2fb3e6</t>
   </si>
   <si>
+    <t>#4D8FD1</t>
+  </si>
+  <si>
+    <t>#4685C2</t>
+  </si>
+  <si>
     <t>#CC0000</t>
   </si>
   <si>
-    <t>#B20000</t>
-  </si>
-  <si>
-    <t>#990000</t>
-  </si>
-  <si>
-    <t>#800000</t>
-  </si>
-  <si>
-    <t>#660000</t>
-  </si>
-  <si>
-    <t>#4D0000</t>
-  </si>
-  <si>
-    <t>#330000</t>
+    <t>#66CC66</t>
+  </si>
+  <si>
+    <t>#5EB85E</t>
+  </si>
+  <si>
+    <t>#a51078</t>
+  </si>
+  <si>
+    <t>#10a588</t>
   </si>
 </sst>
 </file>
@@ -685,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81AEE3DF-90D0-4755-BF14-7AE2CA398B23}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -697,7 +697,9 @@
     <col min="4" max="4" width="27.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38.81640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="1"/>
+    <col min="7" max="7" width="9" style="1"/>
+    <col min="8" max="8" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -1095,7 +1097,7 @@
         <v>15</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -1121,7 +1123,7 @@
         <v>16</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -1147,7 +1149,7 @@
         <v>17</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1172,8 +1174,8 @@
       <c r="G19" s="2">
         <v>18</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>88</v>
+      <c r="H19" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -1198,8 +1200,8 @@
       <c r="G20" s="1">
         <v>19</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>89</v>
+      <c r="H20" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Enhance 3D Gun Barrel Plot functionality by adding New Mexico land survey system support, increasing plot size, and updating workflow tasks
</commit_message>
<xml_diff>
--- a/app/database/stratigraphic.xlsx
+++ b/app/database/stratigraphic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\steve\projects\afe\app\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA97429-190B-4176-B60A-1CDB5FDE681B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEFF6C5-054E-4852-957D-51CD58BA86EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{5A26212E-1421-4DA3-B8E9-B09BBE008E54}"/>
+    <workbookView xWindow="960" yWindow="2250" windowWidth="24000" windowHeight="14390" xr2:uid="{5A26212E-1421-4DA3-B8E9-B09BBE008E54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -287,9 +287,6 @@
     <t>#2fb3e6</t>
   </si>
   <si>
-    <t>#4D8FD1</t>
-  </si>
-  <si>
     <t>#4685C2</t>
   </si>
   <si>
@@ -299,13 +296,16 @@
     <t>#66CC66</t>
   </si>
   <si>
-    <t>#5EB85E</t>
-  </si>
-  <si>
     <t>#a51078</t>
   </si>
   <si>
     <t>#10a588</t>
+  </si>
+  <si>
+    <t>#D3D3D3</t>
+  </si>
+  <si>
+    <t>#ADD8E6</t>
   </si>
 </sst>
 </file>
@@ -686,7 +686,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1045,7 +1045,7 @@
         <v>13</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -1071,7 +1071,7 @@
         <v>14</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -1097,7 +1097,7 @@
         <v>15</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -1123,7 +1123,7 @@
         <v>16</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -1149,7 +1149,7 @@
         <v>17</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1175,7 +1175,7 @@
         <v>18</v>
       </c>
       <c r="H19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -1201,7 +1201,7 @@
         <v>19</v>
       </c>
       <c r="H20" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add redhills project context and update references in gun barrel plot tasks
</commit_message>
<xml_diff>
--- a/app/database/stratigraphic.xlsx
+++ b/app/database/stratigraphic.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\steve\projects\afe\app\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\ubuntu\afe\repos\afe\app\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEFF6C5-054E-4852-957D-51CD58BA86EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCD3683-1B29-4138-827D-A650A7E19A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="2250" windowWidth="24000" windowHeight="14390" xr2:uid="{5A26212E-1421-4DA3-B8E9-B09BBE008E54}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="89">
   <si>
     <t>Permian</t>
   </si>
@@ -300,9 +300,6 @@
   </si>
   <si>
     <t>#10a588</t>
-  </si>
-  <si>
-    <t>#D3D3D3</t>
   </si>
   <si>
     <t>#ADD8E6</t>
@@ -686,7 +683,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1045,7 +1042,7 @@
         <v>13</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -1201,7 +1198,7 @@
         <v>19</v>
       </c>
       <c r="H20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>